<commit_message>
Added Ant Colony Optimization
</commit_message>
<xml_diff>
--- a/Docs/MA Results.xlsx
+++ b/Docs/MA Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/issackondreddy/Desktop/Education/Projects/Cancer Detection/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8847319D-80F9-AE46-A52C-EF3D6F83968A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4120E505-9251-0049-886E-90BA6EA4C8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{9F405C5C-E1F3-9841-A1DD-6FAEEAF9C47C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Algorithm</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Parameters</t>
   </si>
   <si>
-    <t>Curve Image Path</t>
-  </si>
-  <si>
     <t>Genetic Algorithm</t>
   </si>
   <si>
@@ -75,13 +72,29 @@
   </si>
   <si>
     <t>Rosenbrock</t>
+  </si>
+  <si>
+    <t>Particle Swarm Optimization</t>
+  </si>
+  <si>
+    <t>"Population Size": 100, 
+"Chromosome Length": 30,
+"Crossover Rate": 0.8,
+"Mutation Rate": 0.01,</t>
+  </si>
+  <si>
+    <t>Number of Particles: 30
+Iterations: 100
+c1: 1.49
+c2: 1.49
+w: 0.729</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +107,35 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF080808"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF1750EB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF871094"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="4"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,11 +158,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,25 +512,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4162E453-3832-2A4A-A378-7859CB0F533E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
     <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,39 +552,174 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="3">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1.464</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="F3" s="3">
+        <v>100</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>17.79</v>
+      </c>
+      <c r="D4" s="3">
+        <v>67.959999999999994</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6.34</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>78.064999999999998</v>
+      </c>
+      <c r="D5" s="3">
+        <v>152.91</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20.067</v>
+      </c>
+      <c r="F5" s="3">
+        <v>100</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D6" s="3">
+        <v>20000</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="D7" s="3">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <v>20000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>20000</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9801010201</v>
+      </c>
+      <c r="D9" s="3">
+        <v>9801010201</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A2:A5"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="G6:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Evolutionary Stratagies Algorithm Added
</commit_message>
<xml_diff>
--- a/Docs/MA Results.xlsx
+++ b/Docs/MA Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/issackondreddy/Desktop/Education/Projects/Cancer Detection/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E5B94B-9EFF-AD4A-85EB-70F994D5301E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C7918-D129-E145-AE82-57C3CDD24A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{9F405C5C-E1F3-9841-A1DD-6FAEEAF9C47C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>Algorithm</t>
   </si>
@@ -272,6 +272,15 @@
 'rastrigin': {'initial_temp': 8000, 'final_temp': 1, 'alpha': 0.95, 'max_iterations': 1200},
 'rosenbrock': {'initial_temp': 10000, 'final_temp': 1, 'alpha': 0.97, 'max_iterations': 1500},</t>
     </r>
+  </si>
+  <si>
+    <t>Tabu Search</t>
+  </si>
+  <si>
+    <t>Differential Evolution</t>
+  </si>
+  <si>
+    <t>Evolutionary Strategies</t>
   </si>
 </sst>
 </file>
@@ -372,15 +381,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -391,12 +406,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,6 +422,338 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7032A0D-B7F0-B34F-8876-4515D042C93E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8801100" y="3454400"/>
+          <a:ext cx="3581400" cy="774700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>num_iterations = 100</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>tabu_tenure = 15  # How long moves are forbidden</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>num_neighbors = 50</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="Text Box 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B6EBCA-7A55-D4E7-F542-F17B3AD1B1C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8724900" y="4267200"/>
+          <a:ext cx="3873500" cy="812800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "Population Size": 100,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "Chromosome Length": 30,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "F": 0.8,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "CR": 0.9,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "Generations": 100</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="Text Box 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAE5FB3-7BF5-CFD7-D586-4C324365C8BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8648700" y="5080000"/>
+          <a:ext cx="3987800" cy="825500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>"Population Size": 50,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "Sigma": 0.1,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "Learning Rate": 0.001,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>            "Max Iters": 1000</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4162E453-3832-2A4A-A378-7859CB0F533E}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -775,7 +1116,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
@@ -793,12 +1134,12 @@
       <c r="F2" s="2">
         <v>100</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -814,10 +1155,10 @@
       <c r="F3" s="2">
         <v>100</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5"/>
+      <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -833,10 +1174,10 @@
       <c r="F4" s="2">
         <v>100</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
+      <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -852,10 +1193,10 @@
       <c r="F5" s="2">
         <v>100</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -873,12 +1214,12 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="8"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -894,10 +1235,10 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="8"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -913,10 +1254,10 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="8"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -932,10 +1273,10 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
@@ -953,12 +1294,12 @@
       <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="8"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -974,10 +1315,10 @@
       <c r="F11" s="2">
         <v>0</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="8"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -993,10 +1334,10 @@
       <c r="F12" s="2">
         <v>0</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="8"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -1012,10 +1353,10 @@
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -1033,14 +1374,14 @@
       <c r="F14" s="4">
         <v>0</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="8"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -1056,12 +1397,12 @@
       <c r="F15" s="4">
         <v>0</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="8"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1077,12 +1418,12 @@
       <c r="F16" s="4">
         <v>0</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="8"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -1098,21 +1439,273 @@
       <c r="F17" s="4">
         <v>0</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4257.6000000000004</v>
+      </c>
+      <c r="D18" s="2">
+        <v>10597.2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>16406.669999999998</v>
+      </c>
+      <c r="F18" s="2">
+        <v>90</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2">
+        <v>21.08</v>
+      </c>
+      <c r="D19" s="2">
+        <v>21.09</v>
+      </c>
+      <c r="E19" s="2">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>94</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5"/>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4895.0600000000004</v>
+      </c>
+      <c r="D20" s="2">
+        <v>11057.11</v>
+      </c>
+      <c r="E20" s="2">
+        <v>17569.599999999999</v>
+      </c>
+      <c r="F20" s="2">
+        <v>91</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="5"/>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>143459275.71000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3296981520.4050002</v>
+      </c>
+      <c r="E21" s="2">
+        <v>11262550553.75</v>
+      </c>
+      <c r="F21" s="2">
+        <v>76</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6.056</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9.7330000000000005</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3.43</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.8210000000000002</v>
+      </c>
+      <c r="E23" s="2">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2">
+        <v>206.72800000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>263.02</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="F24" s="2">
+        <v>90</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="5"/>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2">
+        <v>728.69</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1433.6549</v>
+      </c>
+      <c r="E25" s="2">
+        <v>27.91</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2">
+        <v>6906.68</v>
+      </c>
+      <c r="D26" s="2">
+        <v>42743.68</v>
+      </c>
+      <c r="E26" s="2">
+        <v>25848.33</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="2">
+        <v>20.18</v>
+      </c>
+      <c r="D27" s="2">
+        <v>20.25</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.113</v>
+      </c>
+      <c r="F27" s="2">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2">
+        <v>17497.313999999998</v>
+      </c>
+      <c r="D28" s="2">
+        <v>52088.93</v>
+      </c>
+      <c r="E28" s="3">
+        <v>25165.25</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="5"/>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="2">
+        <v>682181818.29999995</v>
+      </c>
+      <c r="D29" s="2">
+        <v>19213636477.48</v>
+      </c>
+      <c r="E29" s="2">
+        <v>18845633637.68</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="G14:I17"/>
+  <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="G10:G13"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="G18:I21"/>
+    <mergeCell ref="G22:I25"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="G14:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Whale optimization Algorithm
</commit_message>
<xml_diff>
--- a/Docs/MA Results.xlsx
+++ b/Docs/MA Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/issackondreddy/Desktop/Education/Projects/Cancer Detection/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5BE2D0-9DCE-D44B-8369-1D1278381F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F375CFFD-6B3B-E342-960C-418B9B35AB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{9F405C5C-E1F3-9841-A1DD-6FAEEAF9C47C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
   <si>
     <t>Algorithm</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>Firefly Algorithm</t>
+  </si>
+  <si>
+    <t>Whale Optimization Algorithm</t>
   </si>
 </sst>
 </file>
@@ -879,6 +882,76 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="Text Box 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A65CAC-F748-DA58-A3B8-ACC986E651FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8648700" y="7518400"/>
+          <a:ext cx="2273300" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1100"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Aptos Narrow" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>whales_no=30, iterations=100, b=1,lb, ub, dim = -100, 100, 30</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1199,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4162E453-3832-2A4A-A378-7859CB0F533E}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:G33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1969,12 +2042,87 @@
         <v>31</v>
       </c>
     </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1.67523</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3252.6869999999999</v>
+      </c>
+      <c r="E38" s="2">
+        <v>11379.665999999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="5"/>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5.36</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="E39" s="2">
+        <v>7.6059999999999999</v>
+      </c>
+      <c r="F39" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="5"/>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2.1080000000000001</v>
+      </c>
+      <c r="D40" s="2">
+        <v>3578.97</v>
+      </c>
+      <c r="E40" s="2">
+        <v>12824.58</v>
+      </c>
+      <c r="F40" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="5"/>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="2">
+        <v>28.76</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2344970766.1329999</v>
+      </c>
+      <c r="E41" s="2">
+        <v>7505828997.6599998</v>
+      </c>
+      <c r="F41" s="2">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="G30:G33"/>
     <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A41"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="G2:G5"/>
     <mergeCell ref="A6:A9"/>

</xml_diff>

<commit_message>
Completed all 20 Metaheuristic Algorithms
</commit_message>
<xml_diff>
--- a/Docs/MA Results.xlsx
+++ b/Docs/MA Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/issackondreddy/Desktop/Education/Projects/Cancer Detection/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F375CFFD-6B3B-E342-960C-418B9B35AB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDD47C9-8D87-6241-BDB6-8B5C65D744BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15680" xr2:uid="{9F405C5C-E1F3-9841-A1DD-6FAEEAF9C47C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="44">
   <si>
     <t>Algorithm</t>
   </si>
@@ -341,12 +341,100 @@
   <si>
     <t>Whale Optimization Algorithm</t>
   </si>
+  <si>
+    <t>BAT Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Population Size": 100,
+            "Dimension": 30,
+            "Pulse Rate": 0.5,
+            "Loudness": 0.5,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>CS Algorithm</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "pa": 0.25,
+            "alpha": 0.5,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>Dragonfly Algorithm</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "Step Size": 0.1,
+            "Attraction Coefficient": 0.1,
+            "Mutation Probability": 0.05,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>Flower Pollination</t>
+  </si>
+  <si>
+    <t>Harmony Search Algorithm</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "Harmony Memory Size": 20,
+            "Pitch Adjustment Rate": 0.7,
+            "Bandwidth": 0.05,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>Moth_Flame_Optimization</t>
+  </si>
+  <si>
+    <t>Salp swarm Algorithm</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "Step Size": 0.1,
+            "Influence Coefficient": 0.1,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>Grasshopper Optimization Algorithm</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "Step Size": 0.1,
+            "Attraction Coefficient": 0.1,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>Sine Cosine Algorithm</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "Parameter a": 3,
+            "Parameter r": 1,
+            "Generations": 100</t>
+  </si>
+  <si>
+    <t>Biogeography Based Optimizer</t>
+  </si>
+  <si>
+    <t>"Population Size": 100,
+            "Dimension": 30,
+            "Migration Rate": 0.1,
+            "Mutation Rate": 0.05,
+            "Generations": 100</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -412,6 +500,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -433,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -469,6 +563,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,8 +603,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -517,7 +624,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="8801100" y="3454400"/>
-          <a:ext cx="3581400" cy="774700"/>
+          <a:ext cx="3860800" cy="774700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -891,9 +998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1231900</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -911,7 +1018,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="8648700" y="7518400"/>
-          <a:ext cx="2273300" cy="685800"/>
+          <a:ext cx="3111500" cy="838200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1272,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4162E453-3832-2A4A-A378-7859CB0F533E}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="J26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2116,8 +2223,828 @@
         <v>97</v>
       </c>
     </row>
+    <row r="42" spans="1:7" ht="16" customHeight="1">
+      <c r="A42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="15">
+        <v>99.656396212023694</v>
+      </c>
+      <c r="D42" s="15">
+        <v>162.19291086091999</v>
+      </c>
+      <c r="E42" s="15">
+        <v>5.8900206098194996</v>
+      </c>
+      <c r="F42" s="15">
+        <v>100</v>
+      </c>
+      <c r="G42" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="8"/>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="15">
+        <v>7.3583772905380398</v>
+      </c>
+      <c r="D43" s="15">
+        <v>9.1224306342807697</v>
+      </c>
+      <c r="E43" s="15">
+        <v>3.4123226910374102E-2</v>
+      </c>
+      <c r="F43" s="15">
+        <v>100</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="8"/>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="15">
+        <v>342.852271726276</v>
+      </c>
+      <c r="D44" s="15">
+        <v>444.38076085711998</v>
+      </c>
+      <c r="E44" s="15">
+        <v>6.3180047545669797</v>
+      </c>
+      <c r="F44" s="15">
+        <v>100</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="8"/>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="15">
+        <v>60358.147296780298</v>
+      </c>
+      <c r="D45" s="15">
+        <v>200836.81456202199</v>
+      </c>
+      <c r="E45" s="15">
+        <v>14969.9783542243</v>
+      </c>
+      <c r="F45" s="15">
+        <v>100</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="15">
+        <v>120.845333346316</v>
+      </c>
+      <c r="D46" s="15">
+        <v>220.16456232274899</v>
+      </c>
+      <c r="E46" s="15">
+        <v>4.1982450354393199</v>
+      </c>
+      <c r="F46" s="15">
+        <v>25</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="8"/>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="15">
+        <v>8.5585171494975008</v>
+      </c>
+      <c r="D47" s="15">
+        <v>9.9745097075725599</v>
+      </c>
+      <c r="E47" s="15">
+        <v>3.19964832644049E-2</v>
+      </c>
+      <c r="F47" s="15">
+        <v>21</v>
+      </c>
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="8"/>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="15">
+        <v>352.19759378617601</v>
+      </c>
+      <c r="D48" s="15">
+        <v>471.63741122195597</v>
+      </c>
+      <c r="E48" s="15">
+        <v>4.8531937187985799</v>
+      </c>
+      <c r="F48" s="15">
+        <v>35</v>
+      </c>
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="8"/>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="15">
+        <v>151320.57684429601</v>
+      </c>
+      <c r="D49" s="15">
+        <v>366071.07462628098</v>
+      </c>
+      <c r="E49" s="15">
+        <v>3095.5646763507498</v>
+      </c>
+      <c r="F49" s="15">
+        <v>11</v>
+      </c>
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="15">
+        <v>20.9376635326886</v>
+      </c>
+      <c r="D50" s="15">
+        <v>102.59748759285399</v>
+      </c>
+      <c r="E50" s="15">
+        <v>3.01268565952414</v>
+      </c>
+      <c r="F50" s="15">
+        <v>100</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="8"/>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="15">
+        <v>4.8724200360808201</v>
+      </c>
+      <c r="D51" s="15">
+        <v>8.0358289631622402</v>
+      </c>
+      <c r="E51" s="15">
+        <v>7.0718332252752703E-2</v>
+      </c>
+      <c r="F51" s="15">
+        <v>72</v>
+      </c>
+      <c r="G51" s="19"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="8"/>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="15">
+        <v>310.78700934102199</v>
+      </c>
+      <c r="D52" s="15">
+        <v>473.90567177993398</v>
+      </c>
+      <c r="E52" s="15">
+        <v>4.5221705680225099</v>
+      </c>
+      <c r="F52" s="15">
+        <v>21</v>
+      </c>
+      <c r="G52" s="19"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="8"/>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="15">
+        <v>28224.174222750698</v>
+      </c>
+      <c r="D53" s="15">
+        <v>189835.47419234301</v>
+      </c>
+      <c r="E53" s="15">
+        <v>14839.8427886017</v>
+      </c>
+      <c r="F53" s="15">
+        <v>29</v>
+      </c>
+      <c r="G53" s="19"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="15">
+        <v>35.329654951984502</v>
+      </c>
+      <c r="D54" s="15">
+        <v>35.329654951984502</v>
+      </c>
+      <c r="E54" s="15">
+        <v>3.2532975936550099</v>
+      </c>
+      <c r="F54" s="15">
+        <v>44</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="8"/>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="15">
+        <v>5.7301279812958796</v>
+      </c>
+      <c r="D55" s="15">
+        <v>8.1482665978065096</v>
+      </c>
+      <c r="E55" s="15">
+        <v>6.1637150111267698E-2</v>
+      </c>
+      <c r="F55" s="15">
+        <v>42</v>
+      </c>
+      <c r="G55" s="19"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="8"/>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="15">
+        <v>270.135482397126</v>
+      </c>
+      <c r="D56" s="15">
+        <v>414.667267886665</v>
+      </c>
+      <c r="E56" s="15">
+        <v>3.2111996904362501</v>
+      </c>
+      <c r="F56" s="15">
+        <v>52</v>
+      </c>
+      <c r="G56" s="19"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="8"/>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="15">
+        <v>15845.715749874</v>
+      </c>
+      <c r="D57" s="15">
+        <v>123886.508080391</v>
+      </c>
+      <c r="E57" s="15">
+        <v>10731.9979830718</v>
+      </c>
+      <c r="F57" s="15">
+        <v>60</v>
+      </c>
+      <c r="G57" s="19"/>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" s="15">
+        <v>176.60938200471699</v>
+      </c>
+      <c r="D58" s="15">
+        <v>264.63744368096798</v>
+      </c>
+      <c r="E58" s="15">
+        <v>3.01713321876628</v>
+      </c>
+      <c r="F58" s="15">
+        <v>13</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="8"/>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" s="15">
+        <v>9.6424281663405207</v>
+      </c>
+      <c r="D59" s="15">
+        <v>10.634319656872499</v>
+      </c>
+      <c r="E59" s="15">
+        <v>2.76707291480543E-2</v>
+      </c>
+      <c r="F59" s="15">
+        <v>11</v>
+      </c>
+      <c r="G59" s="19"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="8"/>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="15">
+        <v>481.64782893484397</v>
+      </c>
+      <c r="D60" s="15">
+        <v>566.20149682434896</v>
+      </c>
+      <c r="E60" s="15">
+        <v>3.4424884672570899</v>
+      </c>
+      <c r="F60" s="15">
+        <v>14</v>
+      </c>
+      <c r="G60" s="19"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="8"/>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="15">
+        <v>183982.39607078399</v>
+      </c>
+      <c r="D61" s="15">
+        <v>371786.85869179899</v>
+      </c>
+      <c r="E61" s="15">
+        <v>7662.6419004605004</v>
+      </c>
+      <c r="F61" s="15">
+        <v>11</v>
+      </c>
+      <c r="G61" s="19"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" s="15">
+        <v>31.683181644662699</v>
+      </c>
+      <c r="D62" s="15">
+        <v>122.394671888358</v>
+      </c>
+      <c r="E62" s="15">
+        <v>4.2829914223045096</v>
+      </c>
+      <c r="F62" s="15">
+        <v>60</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="8"/>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="15">
+        <v>5.58483747172059</v>
+      </c>
+      <c r="D63" s="15">
+        <v>8.2604946166298596</v>
+      </c>
+      <c r="E63" s="15">
+        <v>0.107327752520121</v>
+      </c>
+      <c r="F63" s="15">
+        <v>59</v>
+      </c>
+      <c r="G63" s="19"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="8"/>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="15">
+        <v>275.22530904886702</v>
+      </c>
+      <c r="D64" s="15">
+        <v>446.59446127271701</v>
+      </c>
+      <c r="E64" s="15">
+        <v>4.2173984582747304</v>
+      </c>
+      <c r="F64" s="15">
+        <v>40</v>
+      </c>
+      <c r="G64" s="19"/>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="8"/>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="15">
+        <v>17159.039971270799</v>
+      </c>
+      <c r="D65" s="15">
+        <v>160088.35637154599</v>
+      </c>
+      <c r="E65" s="15">
+        <v>14816.9461986554</v>
+      </c>
+      <c r="F65" s="15">
+        <v>41</v>
+      </c>
+      <c r="G65" s="19"/>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="15">
+        <v>1.4020648794492401</v>
+      </c>
+      <c r="D66" s="15">
+        <v>14.6089800171183</v>
+      </c>
+      <c r="E66" s="15">
+        <v>6.9262681820940601</v>
+      </c>
+      <c r="F66" s="15">
+        <v>75</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="8"/>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="15">
+        <v>2.6627376254130599</v>
+      </c>
+      <c r="D67" s="15">
+        <v>3.51475399510133</v>
+      </c>
+      <c r="E67" s="15">
+        <v>0.16391342470919501</v>
+      </c>
+      <c r="F67" s="15">
+        <v>70</v>
+      </c>
+      <c r="G67" s="19"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="8"/>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="15">
+        <v>175.458757982907</v>
+      </c>
+      <c r="D68" s="15">
+        <v>216.921419172919</v>
+      </c>
+      <c r="E68" s="15">
+        <v>15.9194299343186</v>
+      </c>
+      <c r="F68" s="15">
+        <v>100</v>
+      </c>
+      <c r="G68" s="19"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="8"/>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="15">
+        <v>308.26167392584301</v>
+      </c>
+      <c r="D69" s="15">
+        <v>15254.4064540898</v>
+      </c>
+      <c r="E69" s="15">
+        <v>15937.438368368599</v>
+      </c>
+      <c r="F69" s="15">
+        <v>63</v>
+      </c>
+      <c r="G69" s="19"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="15">
+        <v>3.7062508805160501</v>
+      </c>
+      <c r="D70" s="15">
+        <v>70.976311892087793</v>
+      </c>
+      <c r="E70" s="15">
+        <v>11.907531828903</v>
+      </c>
+      <c r="F70" s="15">
+        <v>36</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="8"/>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="15">
+        <v>2.6984273758067601</v>
+      </c>
+      <c r="D71" s="15">
+        <v>5.6724115793758498</v>
+      </c>
+      <c r="E71" s="15">
+        <v>0.23283920622873999</v>
+      </c>
+      <c r="F71" s="15">
+        <v>41</v>
+      </c>
+      <c r="G71" s="19"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="8"/>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="15">
+        <v>207.017841945409</v>
+      </c>
+      <c r="D72" s="15">
+        <v>392.269588315703</v>
+      </c>
+      <c r="E72" s="15">
+        <v>5.7008649972203402</v>
+      </c>
+      <c r="F72" s="15">
+        <v>28</v>
+      </c>
+      <c r="G72" s="19"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="8"/>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="15">
+        <v>370.93013669243999</v>
+      </c>
+      <c r="D73" s="15">
+        <v>89437.869729190497</v>
+      </c>
+      <c r="E73" s="15">
+        <v>27364.604943127899</v>
+      </c>
+      <c r="F73" s="15">
+        <v>27</v>
+      </c>
+      <c r="G73" s="19"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="15">
+        <v>169.848067593737</v>
+      </c>
+      <c r="D74" s="15">
+        <v>281.88739920487899</v>
+      </c>
+      <c r="E74" s="15">
+        <v>3.8357767950158701</v>
+      </c>
+      <c r="F74" s="15">
+        <v>12</v>
+      </c>
+      <c r="G74" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="8"/>
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="15">
+        <v>10.1130740659426</v>
+      </c>
+      <c r="D75" s="15">
+        <v>10.7515337115086</v>
+      </c>
+      <c r="E75" s="15">
+        <v>1.5332908355854401E-2</v>
+      </c>
+      <c r="F75" s="15">
+        <v>13</v>
+      </c>
+      <c r="G75" s="19"/>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="8"/>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="15">
+        <v>535.95937729330001</v>
+      </c>
+      <c r="D76" s="15">
+        <v>573.25539348304699</v>
+      </c>
+      <c r="E76" s="15">
+        <v>3.4763282605094799</v>
+      </c>
+      <c r="F76" s="15">
+        <v>19</v>
+      </c>
+      <c r="G76" s="19"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="8"/>
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="15">
+        <v>402835.57810715301</v>
+      </c>
+      <c r="D77" s="15">
+        <v>490303.99168263498</v>
+      </c>
+      <c r="E77" s="15">
+        <v>3368.8230426909099</v>
+      </c>
+      <c r="F77" s="15">
+        <v>21</v>
+      </c>
+      <c r="G77" s="19"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="15">
+        <v>145.52146612995401</v>
+      </c>
+      <c r="D78" s="15">
+        <v>250.79939430643199</v>
+      </c>
+      <c r="E78" s="15">
+        <v>2.2314886856806599</v>
+      </c>
+      <c r="F78" s="15">
+        <v>16</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="8"/>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" s="15">
+        <v>8.6566974909829</v>
+      </c>
+      <c r="D79" s="15">
+        <v>10.4303697628301</v>
+      </c>
+      <c r="E79" s="15">
+        <v>2.8422901561177299E-2</v>
+      </c>
+      <c r="F79" s="15">
+        <v>13</v>
+      </c>
+      <c r="G79" s="19"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="8"/>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" s="15">
+        <v>424.93869274940499</v>
+      </c>
+      <c r="D80" s="15">
+        <v>550.06561084870498</v>
+      </c>
+      <c r="E80" s="15">
+        <v>4.02435084953337</v>
+      </c>
+      <c r="F80" s="15">
+        <v>36</v>
+      </c>
+      <c r="G80" s="19"/>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="8"/>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81" s="15">
+        <v>204239.030779397</v>
+      </c>
+      <c r="D81" s="15">
+        <v>389165.64526494802</v>
+      </c>
+      <c r="E81" s="15">
+        <v>6788.9957399642399</v>
+      </c>
+      <c r="F81" s="15">
+        <v>38</v>
+      </c>
+      <c r="G81" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="37">
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="G78:G81"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="G70:G73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="G74:G77"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="G42:G45"/>
+    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="G50:G53"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="G30:G33"/>
@@ -2136,6 +3063,7 @@
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="G14:I17"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>